<commit_message>
both first.txt and myxl.xlsx modified
</commit_message>
<xml_diff>
--- a/myxl.xlsx
+++ b/myxl.xlsx
@@ -40,9 +40,14 @@
     <office:spreadsheet>
       <table:calculation-settings table:automatic-find-labels="false"/>
       <table:table table:name="Sheet1" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>utpal</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>podder</text:p>
+          </table:table-cell>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -55,8 +60,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2021-07-27T11:39:36.107696458</meta:creation-date>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="0" meta:object-count="0"/>
     <meta:generator>LibreOffice/5.1.6.2$Linux_x86 LibreOffice_project/10m0$Build-2</meta:generator>
+    <dc:date>2021-07-27T12:41:39.088553570</dc:date>
+    <meta:editing-duration>PT11S</meta:editing-duration>
+    <meta:editing-cycles>1</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="2" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -67,14 +75,14 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">2257</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">4515</config:config-item>
       <config:config-item config:name="VisibleAreaHeight" config:type="int">451</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
               <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
@@ -130,7 +138,7 @@
       <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">gAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMApgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFCgBEVVBMRVhfT0ZG</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
@@ -141,8 +149,9 @@
       <config:config-item config:name="RasterSubdivisionX" config:type="int">1</config:config-item>
       <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
       <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
     </config:config-item-set>
@@ -247,7 +256,7 @@
           <text:p>
             <text:date style:data-style-name="N2" text:date-value="2021-07-27">00/00/0000</text:date>
             , 
-            <text:time>00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="12:41:27.893600440">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>